<commit_message>
Slight update on the test file.
</commit_message>
<xml_diff>
--- a/test/xlsx/boolean-value/input.xlsx
+++ b/test/xlsx/boolean-value/input.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Boolean value</t>
+    <t>Boolean Value</t>
   </si>
 </sst>
 </file>
@@ -380,9 +380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>